<commit_message>
Automatic code generation for flask api endpoint schema definition notebook added to hackaton IV project
</commit_message>
<xml_diff>
--- a/Conflicts in Brasil Data Analysis/Dados/Dados/ter-serie.xlsx
+++ b/Conflicts in Brasil Data Analysis/Dados/Dados/ter-serie.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L239"/>
+  <dimension ref="A1:L238"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -676,7 +676,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Alta Floresta;Oeste</t>
+          <t>Alta Floresta D'Oeste</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -836,7 +836,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Alvorada;Oeste</t>
+          <t>Alvorada D'Oeste</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -3076,7 +3076,7 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>Conquista;Oeste</t>
+          <t>Conquista D'Oeste</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -3556,7 +3556,7 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>Diamante;Oeste</t>
+          <t>Diamante D'Oeste</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -4356,7 +4356,7 @@
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>Glória;Oeste</t>
+          <t>Glória D'Oeste</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -6356,7 +6356,7 @@
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>Nova Brasilândia;Oeste</t>
+          <t>Nova Brasilândia D'Oeste</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -7156,7 +7156,7 @@
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>Pimenteiras</t>
+          <t>Pimenteiras do Oeste</t>
         </is>
       </c>
       <c r="B169" t="n">
@@ -7187,23 +7187,23 @@
         <v>0</v>
       </c>
       <c r="K169" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L169" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>Pimenteiras do Oeste</t>
+          <t>Planalto</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D170" t="n">
         <v>0</v>
@@ -7227,23 +7227,23 @@
         <v>0</v>
       </c>
       <c r="K170" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>Planalto</t>
+          <t>Plácido de Castro</t>
         </is>
       </c>
       <c r="B171" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C171" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D171" t="n">
         <v>0</v>
@@ -7255,7 +7255,7 @@
         <v>0</v>
       </c>
       <c r="G171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H171" t="n">
         <v>0</v>
@@ -7267,32 +7267,32 @@
         <v>0</v>
       </c>
       <c r="K171" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L171" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>Plácido de Castro</t>
+          <t>Poconé</t>
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C172" t="n">
         <v>0</v>
       </c>
       <c r="D172" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G172" t="n">
         <v>1</v>
@@ -7304,10 +7304,10 @@
         <v>0</v>
       </c>
       <c r="J172" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K172" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L172" t="n">
         <v>4</v>
@@ -7316,54 +7316,54 @@
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>Poconé</t>
+          <t>Ponta Porã</t>
         </is>
       </c>
       <c r="B173" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D173" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E173" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F173" t="n">
         <v>1</v>
       </c>
       <c r="G173" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H173" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J173" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K173" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L173" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>Ponta Porã</t>
+          <t>Pontes e Lacerda</t>
         </is>
       </c>
       <c r="B174" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C174" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D174" t="n">
         <v>0</v>
@@ -7372,47 +7372,47 @@
         <v>0</v>
       </c>
       <c r="F174" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G174" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H174" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I174" t="n">
         <v>1</v>
       </c>
       <c r="J174" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K174" t="n">
         <v>4</v>
       </c>
       <c r="L174" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>Pontes e Lacerda</t>
+          <t>Porto Acre</t>
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C175" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D175" t="n">
         <v>0</v>
       </c>
       <c r="E175" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F175" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G175" t="n">
         <v>1</v>
@@ -7424,35 +7424,35 @@
         <v>1</v>
       </c>
       <c r="J175" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K175" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L175" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>Porto Acre</t>
+          <t>Porto Esperidião</t>
         </is>
       </c>
       <c r="B176" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C176" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D176" t="n">
         <v>0</v>
       </c>
       <c r="E176" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F176" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G176" t="n">
         <v>1</v>
@@ -7464,19 +7464,19 @@
         <v>1</v>
       </c>
       <c r="J176" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K176" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>Porto Esperidião</t>
+          <t>Porto Estrela</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -7492,7 +7492,7 @@
         <v>0</v>
       </c>
       <c r="F177" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G177" t="n">
         <v>1</v>
@@ -7501,22 +7501,22 @@
         <v>0</v>
       </c>
       <c r="I177" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J177" t="n">
         <v>0</v>
       </c>
       <c r="K177" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L177" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>Porto Estrela</t>
+          <t>Porto Grande</t>
         </is>
       </c>
       <c r="B178" t="n">
@@ -7532,10 +7532,10 @@
         <v>0</v>
       </c>
       <c r="F178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G178" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H178" t="n">
         <v>0</v>
@@ -7556,140 +7556,140 @@
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>Porto Grande</t>
+          <t>Porto Murtinho</t>
         </is>
       </c>
       <c r="B179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C179" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D179" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E179" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F179" t="n">
         <v>1</v>
       </c>
       <c r="G179" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I179" t="n">
         <v>0</v>
       </c>
       <c r="J179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K179" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L179" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>Porto Murtinho</t>
+          <t>Porto Velho</t>
         </is>
       </c>
       <c r="B180" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C180" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D180" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E180" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F180" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G180" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H180" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I180" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J180" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="K180" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L180" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>Porto Velho</t>
+          <t>Porto Walter</t>
         </is>
       </c>
       <c r="B181" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C181" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D181" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E181" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F181" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G181" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H181" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I181" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J181" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K181" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="L181" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>Porto Walter</t>
+          <t>Pracuúba</t>
         </is>
       </c>
       <c r="B182" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C182" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D182" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E182" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F182" t="n">
         <v>0</v>
@@ -7704,66 +7704,66 @@
         <v>0</v>
       </c>
       <c r="J182" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K182" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L182" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>Pracuúba</t>
+          <t>Quedas do Iguaçu</t>
         </is>
       </c>
       <c r="B183" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C183" t="n">
+        <v>0</v>
+      </c>
+      <c r="D183" t="n">
+        <v>0</v>
+      </c>
+      <c r="E183" t="n">
+        <v>0</v>
+      </c>
+      <c r="F183" t="n">
+        <v>1</v>
+      </c>
+      <c r="G183" t="n">
+        <v>0</v>
+      </c>
+      <c r="H183" t="n">
+        <v>0</v>
+      </c>
+      <c r="I183" t="n">
+        <v>0</v>
+      </c>
+      <c r="J183" t="n">
+        <v>2</v>
+      </c>
+      <c r="K183" t="n">
+        <v>0</v>
+      </c>
+      <c r="L183" t="n">
         <v>4</v>
-      </c>
-      <c r="D183" t="n">
-        <v>2</v>
-      </c>
-      <c r="E183" t="n">
-        <v>3</v>
-      </c>
-      <c r="F183" t="n">
-        <v>0</v>
-      </c>
-      <c r="G183" t="n">
-        <v>0</v>
-      </c>
-      <c r="H183" t="n">
-        <v>0</v>
-      </c>
-      <c r="I183" t="n">
-        <v>0</v>
-      </c>
-      <c r="J183" t="n">
-        <v>5</v>
-      </c>
-      <c r="K183" t="n">
-        <v>0</v>
-      </c>
-      <c r="L183" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>Quedas do Iguaçu</t>
+          <t>Realeza</t>
         </is>
       </c>
       <c r="B184" t="n">
         <v>1</v>
       </c>
       <c r="C184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D184" t="n">
         <v>0</v>
@@ -7772,7 +7772,7 @@
         <v>0</v>
       </c>
       <c r="F184" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G184" t="n">
         <v>0</v>
@@ -7784,26 +7784,26 @@
         <v>0</v>
       </c>
       <c r="J184" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K184" t="n">
         <v>0</v>
       </c>
       <c r="L184" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>Realeza</t>
+          <t>Redentora</t>
         </is>
       </c>
       <c r="B185" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C185" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D185" t="n">
         <v>0</v>
@@ -7821,22 +7821,22 @@
         <v>0</v>
       </c>
       <c r="I185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J185" t="n">
         <v>0</v>
       </c>
       <c r="K185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>Redentora</t>
+          <t>Rio Bonito do Iguaçu</t>
         </is>
       </c>
       <c r="B186" t="n">
@@ -7861,149 +7861,149 @@
         <v>0</v>
       </c>
       <c r="I186" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J186" t="n">
         <v>0</v>
       </c>
       <c r="K186" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L186" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>Rio Bonito do Iguaçu</t>
+          <t>Rio Branco</t>
         </is>
       </c>
       <c r="B187" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C187" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D187" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E187" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F187" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G187" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H187" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="I187" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="J187" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="K187" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L187" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>Rio Branco</t>
+          <t>Rio Brilhante</t>
         </is>
       </c>
       <c r="B188" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C188" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D188" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E188" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F188" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G188" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="H188" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="I188" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="J188" t="n">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="K188" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L188" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>Rio Brilhante</t>
+          <t>Rodrigues Alves</t>
         </is>
       </c>
       <c r="B189" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C189" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D189" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E189" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F189" t="n">
         <v>0</v>
       </c>
       <c r="G189" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H189" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I189" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K189" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>Rodrigues Alves</t>
+          <t>Rolim de Moura</t>
         </is>
       </c>
       <c r="B190" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C190" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D190" t="n">
         <v>0</v>
@@ -8015,38 +8015,38 @@
         <v>0</v>
       </c>
       <c r="G190" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H190" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I190" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J190" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K190" t="n">
         <v>2</v>
       </c>
       <c r="L190" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>Rolim de Moura</t>
+          <t>Ronda Alta</t>
         </is>
       </c>
       <c r="B191" t="n">
         <v>0</v>
       </c>
       <c r="C191" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E191" t="n">
         <v>0</v>
@@ -8055,7 +8055,7 @@
         <v>0</v>
       </c>
       <c r="G191" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H191" t="n">
         <v>1</v>
@@ -8064,29 +8064,29 @@
         <v>0</v>
       </c>
       <c r="J191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K191" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L191" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>Ronda Alta</t>
+          <t>Rorainópolis</t>
         </is>
       </c>
       <c r="B192" t="n">
         <v>0</v>
       </c>
       <c r="C192" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D192" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E192" t="n">
         <v>0</v>
@@ -8104,19 +8104,19 @@
         <v>0</v>
       </c>
       <c r="J192" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K192" t="n">
         <v>0</v>
       </c>
       <c r="L192" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>Rorainópolis</t>
+          <t>Salto do Céu</t>
         </is>
       </c>
       <c r="B193" t="n">
@@ -8132,7 +8132,7 @@
         <v>0</v>
       </c>
       <c r="F193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G193" t="n">
         <v>0</v>
@@ -8144,26 +8144,26 @@
         <v>0</v>
       </c>
       <c r="J193" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K193" t="n">
         <v>0</v>
       </c>
       <c r="L193" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>Salto do Céu</t>
+          <t>Sant'Ana do Livramento</t>
         </is>
       </c>
       <c r="B194" t="n">
         <v>0</v>
       </c>
       <c r="C194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D194" t="n">
         <v>0</v>
@@ -8172,13 +8172,13 @@
         <v>0</v>
       </c>
       <c r="F194" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G194" t="n">
         <v>0</v>
       </c>
       <c r="H194" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I194" t="n">
         <v>0</v>
@@ -8196,17 +8196,17 @@
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>Sant&amp;#39;Ana do Livramento</t>
+          <t>Santa Helena</t>
         </is>
       </c>
       <c r="B195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C195" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E195" t="n">
         <v>0</v>
@@ -8215,32 +8215,32 @@
         <v>0</v>
       </c>
       <c r="G195" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I195" t="n">
         <v>0</v>
       </c>
       <c r="J195" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K195" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>Santa Helena</t>
+          <t>Santa Isabel do Rio Negro</t>
         </is>
       </c>
       <c r="B196" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C196" t="n">
         <v>0</v>
@@ -8255,38 +8255,38 @@
         <v>0</v>
       </c>
       <c r="G196" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H196" t="n">
         <v>1</v>
       </c>
       <c r="I196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J196" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K196" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L196" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>Santa Isabel do Rio Negro</t>
+          <t>Santa Maria</t>
         </is>
       </c>
       <c r="B197" t="n">
         <v>0</v>
       </c>
       <c r="C197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D197" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E197" t="n">
         <v>0</v>
@@ -8298,10 +8298,10 @@
         <v>0</v>
       </c>
       <c r="H197" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I197" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J197" t="n">
         <v>0</v>
@@ -8316,20 +8316,20 @@
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>Santa Maria</t>
+          <t>Santa Rosa do Purus</t>
         </is>
       </c>
       <c r="B198" t="n">
         <v>0</v>
       </c>
       <c r="C198" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D198" t="n">
         <v>0</v>
       </c>
       <c r="E198" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F198" t="n">
         <v>0</v>
@@ -8347,7 +8347,7 @@
         <v>0</v>
       </c>
       <c r="K198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L198" t="n">
         <v>0</v>
@@ -8356,7 +8356,7 @@
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>Santa Rosa do Purus</t>
+          <t>Santa Terezinha de Itaipu</t>
         </is>
       </c>
       <c r="B199" t="n">
@@ -8369,7 +8369,7 @@
         <v>0</v>
       </c>
       <c r="E199" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F199" t="n">
         <v>0</v>
@@ -8384,10 +8384,10 @@
         <v>0</v>
       </c>
       <c r="J199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K199" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L199" t="n">
         <v>0</v>
@@ -8396,7 +8396,7 @@
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>Santa Terezinha de Itaipu</t>
+          <t>Santo Antônio do Içá</t>
         </is>
       </c>
       <c r="B200" t="n">
@@ -8409,7 +8409,7 @@
         <v>0</v>
       </c>
       <c r="E200" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F200" t="n">
         <v>0</v>
@@ -8418,10 +8418,10 @@
         <v>0</v>
       </c>
       <c r="H200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I200" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J200" t="n">
         <v>1</v>
@@ -8436,7 +8436,7 @@
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>Santo Antônio do Içá</t>
+          <t>Sapezal</t>
         </is>
       </c>
       <c r="B201" t="n">
@@ -8446,10 +8446,10 @@
         <v>0</v>
       </c>
       <c r="D201" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F201" t="n">
         <v>0</v>
@@ -8458,16 +8458,16 @@
         <v>0</v>
       </c>
       <c r="H201" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I201" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J201" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K201" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L201" t="n">
         <v>0</v>
@@ -8476,7 +8476,7 @@
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>Sapezal</t>
+          <t>Sarandi</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -8486,13 +8486,13 @@
         <v>0</v>
       </c>
       <c r="D202" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E202" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F202" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G202" t="n">
         <v>0</v>
@@ -8501,13 +8501,13 @@
         <v>0</v>
       </c>
       <c r="I202" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J202" t="n">
         <v>0</v>
       </c>
       <c r="K202" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L202" t="n">
         <v>0</v>
@@ -8516,7 +8516,7 @@
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>Sarandi</t>
+          <t>Saudades</t>
         </is>
       </c>
       <c r="B203" t="n">
@@ -8532,7 +8532,7 @@
         <v>0</v>
       </c>
       <c r="F203" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G203" t="n">
         <v>0</v>
@@ -8544,10 +8544,10 @@
         <v>0</v>
       </c>
       <c r="J203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L203" t="n">
         <v>0</v>
@@ -8556,7 +8556,7 @@
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>Saudades</t>
+          <t>Seara</t>
         </is>
       </c>
       <c r="B204" t="n">
@@ -8596,7 +8596,7 @@
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>Seara</t>
+          <t>Sena Madureira</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -8609,34 +8609,34 @@
         <v>0</v>
       </c>
       <c r="E205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F205" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G205" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I205" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J205" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K205" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L205" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>Sena Madureira</t>
+          <t>Senador Guiomard</t>
         </is>
       </c>
       <c r="B206" t="n">
@@ -8646,148 +8646,148 @@
         <v>0</v>
       </c>
       <c r="D206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E206" t="n">
         <v>1</v>
       </c>
       <c r="F206" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G206" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H206" t="n">
         <v>1</v>
       </c>
       <c r="I206" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J206" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K206" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L206" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>Senador Guiomard</t>
+          <t>Seringueiras</t>
         </is>
       </c>
       <c r="B207" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C207" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D207" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E207" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F207" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G207" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H207" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I207" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J207" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K207" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="L207" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>Seringueiras</t>
+          <t>Serra do Navio</t>
         </is>
       </c>
       <c r="B208" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C208" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D208" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E208" t="n">
         <v>8</v>
       </c>
       <c r="F208" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G208" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H208" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I208" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J208" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K208" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="L208" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>Serra do Navio</t>
+          <t>Sete Quedas</t>
         </is>
       </c>
       <c r="B209" t="n">
         <v>0</v>
       </c>
       <c r="C209" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D209" t="n">
         <v>0</v>
       </c>
       <c r="E209" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F209" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G209" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H209" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K209" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L209" t="n">
         <v>0</v>
@@ -8796,23 +8796,23 @@
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>Sete Quedas</t>
+          <t>Sidrolândia</t>
         </is>
       </c>
       <c r="B210" t="n">
         <v>0</v>
       </c>
       <c r="C210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D210" t="n">
         <v>0</v>
       </c>
       <c r="E210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F210" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G210" t="n">
         <v>0</v>
@@ -8821,38 +8821,38 @@
         <v>0</v>
       </c>
       <c r="I210" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J210" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K210" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>Sidrolândia</t>
+          <t>São Borja</t>
         </is>
       </c>
       <c r="B211" t="n">
         <v>0</v>
       </c>
       <c r="C211" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D211" t="n">
         <v>0</v>
       </c>
       <c r="E211" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F211" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G211" t="n">
         <v>0</v>
@@ -8864,109 +8864,109 @@
         <v>0</v>
       </c>
       <c r="J211" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K211" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L211" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>São Borja</t>
+          <t>São Francisco do Guaporé</t>
         </is>
       </c>
       <c r="B212" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C212" t="n">
         <v>2</v>
       </c>
       <c r="D212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E212" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F212" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G212" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H212" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J212" t="n">
         <v>0</v>
       </c>
       <c r="K212" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>São Francisco do Guaporé</t>
+          <t>São Gabriel</t>
         </is>
       </c>
       <c r="B213" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C213" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D213" t="n">
         <v>1</v>
       </c>
       <c r="E213" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F213" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G213" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H213" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I213" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J213" t="n">
         <v>0</v>
       </c>
       <c r="K213" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L213" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>São Gabriel</t>
+          <t>São Gabriel da Cachoeira</t>
         </is>
       </c>
       <c r="B214" t="n">
         <v>0</v>
       </c>
       <c r="C214" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D214" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E214" t="n">
         <v>0</v>
@@ -8978,25 +8978,25 @@
         <v>0</v>
       </c>
       <c r="H214" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I214" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J214" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K214" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L214" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>São Gabriel da Cachoeira</t>
+          <t>São José dos Quatro Marcos</t>
         </is>
       </c>
       <c r="B215" t="n">
@@ -9006,7 +9006,7 @@
         <v>0</v>
       </c>
       <c r="D215" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E215" t="n">
         <v>0</v>
@@ -9018,32 +9018,32 @@
         <v>0</v>
       </c>
       <c r="H215" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I215" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J215" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K215" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L215" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>São José dos Quatro Marcos</t>
+          <t>São João da Baliza</t>
         </is>
       </c>
       <c r="B216" t="n">
         <v>0</v>
       </c>
       <c r="C216" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D216" t="n">
         <v>1</v>
@@ -9064,32 +9064,32 @@
         <v>0</v>
       </c>
       <c r="J216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K216" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>São João da Baliza</t>
+          <t>São Lourenço do Sul</t>
         </is>
       </c>
       <c r="B217" t="n">
         <v>0</v>
       </c>
       <c r="C217" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D217" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E217" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F217" t="n">
         <v>0</v>
@@ -9104,32 +9104,32 @@
         <v>0</v>
       </c>
       <c r="J217" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K217" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L217" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>São Lourenço do Sul</t>
+          <t>São Luiz</t>
         </is>
       </c>
       <c r="B218" t="n">
         <v>0</v>
       </c>
       <c r="C218" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D218" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E218" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F218" t="n">
         <v>0</v>
@@ -9144,10 +9144,10 @@
         <v>0</v>
       </c>
       <c r="J218" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K218" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L218" t="n">
         <v>0</v>
@@ -9156,51 +9156,51 @@
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>São Luiz</t>
+          <t>São Miguel do Guaporé</t>
         </is>
       </c>
       <c r="B219" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C219" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D219" t="n">
         <v>1</v>
       </c>
       <c r="E219" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F219" t="n">
         <v>0</v>
       </c>
       <c r="G219" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H219" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I219" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J219" t="n">
         <v>1</v>
       </c>
       <c r="K219" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L219" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>São Miguel do Guaporé</t>
+          <t>São Miguel do Iguaçu</t>
         </is>
       </c>
       <c r="B220" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C220" t="n">
         <v>0</v>
@@ -9209,38 +9209,38 @@
         <v>1</v>
       </c>
       <c r="E220" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F220" t="n">
         <v>0</v>
       </c>
       <c r="G220" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H220" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I220" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J220" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K220" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L220" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>São Miguel do Iguaçu</t>
+          <t>São Paulo de Olivença</t>
         </is>
       </c>
       <c r="B221" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C221" t="n">
         <v>0</v>
@@ -9249,84 +9249,84 @@
         <v>1</v>
       </c>
       <c r="E221" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F221" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I221" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J221" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K221" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L221" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>São Paulo de Olivença</t>
+          <t>Tabatinga</t>
         </is>
       </c>
       <c r="B222" t="n">
         <v>0</v>
       </c>
       <c r="C222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D222" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E222" t="n">
         <v>2</v>
       </c>
       <c r="F222" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G222" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H222" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I222" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J222" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K222" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L222" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>Tabatinga</t>
+          <t>Tacuru</t>
         </is>
       </c>
       <c r="B223" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C223" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D223" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E223" t="n">
         <v>2</v>
@@ -9335,19 +9335,19 @@
         <v>1</v>
       </c>
       <c r="G223" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H223" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I223" t="n">
         <v>2</v>
       </c>
       <c r="J223" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K223" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L223" t="n">
         <v>0</v>
@@ -9356,47 +9356,47 @@
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>Tacuru</t>
+          <t>Tangará da Serra</t>
         </is>
       </c>
       <c r="B224" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C224" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D224" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E224" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F224" t="n">
         <v>1</v>
       </c>
       <c r="G224" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H224" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I224" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J224" t="n">
         <v>0</v>
       </c>
       <c r="K224" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L224" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>Tangará da Serra</t>
+          <t>Tarauacá</t>
         </is>
       </c>
       <c r="B225" t="n">
@@ -9412,31 +9412,31 @@
         <v>0</v>
       </c>
       <c r="F225" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G225" t="n">
         <v>0</v>
       </c>
       <c r="H225" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I225" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J225" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K225" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L225" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>Tarauacá</t>
+          <t>Tenente Portela</t>
         </is>
       </c>
       <c r="B226" t="n">
@@ -9458,16 +9458,16 @@
         <v>0</v>
       </c>
       <c r="H226" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I226" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J226" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K226" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L226" t="n">
         <v>1</v>
@@ -9476,38 +9476,38 @@
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>Tenente Portela</t>
+          <t>Terra Roxa</t>
         </is>
       </c>
       <c r="B227" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C227" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D227" t="n">
         <v>0</v>
       </c>
       <c r="E227" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F227" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G227" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H227" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I227" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J227" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K227" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="L227" t="n">
         <v>1</v>
@@ -9516,57 +9516,57 @@
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>Terra Roxa</t>
+          <t>Tonantins</t>
         </is>
       </c>
       <c r="B228" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C228" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D228" t="n">
         <v>0</v>
       </c>
       <c r="E228" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F228" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G228" t="n">
+        <v>0</v>
+      </c>
+      <c r="H228" t="n">
+        <v>1</v>
+      </c>
+      <c r="I228" t="n">
+        <v>3</v>
+      </c>
+      <c r="J228" t="n">
         <v>6</v>
       </c>
-      <c r="H228" t="n">
-        <v>5</v>
-      </c>
-      <c r="I228" t="n">
-        <v>3</v>
-      </c>
-      <c r="J228" t="n">
-        <v>7</v>
-      </c>
       <c r="K228" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L228" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>Tonantins</t>
+          <t>Três Palmeiras</t>
         </is>
       </c>
       <c r="B229" t="n">
         <v>0</v>
       </c>
       <c r="C229" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D229" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E229" t="n">
         <v>0</v>
@@ -9581,29 +9581,29 @@
         <v>1</v>
       </c>
       <c r="I229" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J229" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K229" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L229" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>Três Palmeiras</t>
+          <t>Tupanciretã</t>
         </is>
       </c>
       <c r="B230" t="n">
         <v>0</v>
       </c>
       <c r="C230" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D230" t="n">
         <v>1</v>
@@ -9618,29 +9618,29 @@
         <v>0</v>
       </c>
       <c r="H230" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I230" t="n">
         <v>0</v>
       </c>
       <c r="J230" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K230" t="n">
         <v>0</v>
       </c>
       <c r="L230" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>Tupanciretã</t>
+          <t>Uiramutã</t>
         </is>
       </c>
       <c r="B231" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C231" t="n">
         <v>0</v>
@@ -9649,34 +9649,34 @@
         <v>1</v>
       </c>
       <c r="E231" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F231" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G231" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H231" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I231" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J231" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K231" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L231" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>Uiramutã</t>
+          <t>Vicente Dutra</t>
         </is>
       </c>
       <c r="B232" t="n">
@@ -9689,44 +9689,44 @@
         <v>1</v>
       </c>
       <c r="E232" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F232" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G232" t="n">
         <v>1</v>
       </c>
       <c r="H232" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I232" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J232" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K232" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L232" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>Vicente Dutra</t>
+          <t>Vicentina</t>
         </is>
       </c>
       <c r="B233" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C233" t="n">
         <v>0</v>
       </c>
       <c r="D233" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E233" t="n">
         <v>0</v>
@@ -9735,10 +9735,10 @@
         <v>0</v>
       </c>
       <c r="G233" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H233" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I233" t="n">
         <v>0</v>
@@ -9756,7 +9756,7 @@
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>Vicentina</t>
+          <t>Vila Bela da Santíssima Trindade</t>
         </is>
       </c>
       <c r="B234" t="n">
@@ -9772,62 +9772,62 @@
         <v>0</v>
       </c>
       <c r="F234" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H234" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I234" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J234" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K234" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="L234" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>Vila Bela da Santíssima Trindade</t>
+          <t>Vilhena</t>
         </is>
       </c>
       <c r="B235" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C235" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D235" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E235" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F235" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G235" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H235" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I235" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J235" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="K235" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L235" t="n">
         <v>4</v>
@@ -9836,78 +9836,78 @@
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>Vilhena</t>
+          <t>Xanxerê</t>
         </is>
       </c>
       <c r="B236" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C236" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D236" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E236" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F236" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G236" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H236" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I236" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J236" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K236" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="L236" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>Xanxerê</t>
+          <t>Xapuri</t>
         </is>
       </c>
       <c r="B237" t="n">
         <v>0</v>
       </c>
       <c r="C237" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D237" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E237" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F237" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G237" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H237" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I237" t="n">
         <v>0</v>
       </c>
       <c r="J237" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K237" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L237" t="n">
         <v>0</v>
@@ -9916,7 +9916,7 @@
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>Xapuri</t>
+          <t>Óbidos</t>
         </is>
       </c>
       <c r="B238" t="n">
@@ -9926,70 +9926,30 @@
         <v>0</v>
       </c>
       <c r="D238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E238" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F238" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G238" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H238" t="n">
         <v>0</v>
       </c>
       <c r="I238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J238" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K238" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L238" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" s="1" t="inlineStr">
-        <is>
-          <t>Óbidos</t>
-        </is>
-      </c>
-      <c r="B239" t="n">
-        <v>0</v>
-      </c>
-      <c r="C239" t="n">
-        <v>0</v>
-      </c>
-      <c r="D239" t="n">
-        <v>1</v>
-      </c>
-      <c r="E239" t="n">
-        <v>4</v>
-      </c>
-      <c r="F239" t="n">
-        <v>2</v>
-      </c>
-      <c r="G239" t="n">
-        <v>2</v>
-      </c>
-      <c r="H239" t="n">
-        <v>0</v>
-      </c>
-      <c r="I239" t="n">
-        <v>1</v>
-      </c>
-      <c r="J239" t="n">
-        <v>0</v>
-      </c>
-      <c r="K239" t="n">
-        <v>6</v>
-      </c>
-      <c r="L239" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>